<commit_message>
Cumulative target and sales added
</commit_message>
<xml_diff>
--- a/Data/Sales_and_Stock.xlsx
+++ b/Data/Sales_and_Stock.xlsx
@@ -1436,10 +1436,10 @@
         <v>154</v>
       </c>
       <c r="G6">
-        <v>7059</v>
+        <v>7060</v>
       </c>
       <c r="H6">
-        <v>7059</v>
+        <v>7060</v>
       </c>
       <c r="I6">
         <v>5460</v>
@@ -1746,10 +1746,10 @@
         <v>28</v>
       </c>
       <c r="G8">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H8">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I8">
         <v>894</v>
@@ -2831,10 +2831,10 @@
         <v>151</v>
       </c>
       <c r="G15">
-        <v>6305</v>
+        <v>6306</v>
       </c>
       <c r="H15">
-        <v>6305</v>
+        <v>6306</v>
       </c>
       <c r="I15">
         <v>5256</v>
@@ -3141,10 +3141,10 @@
         <v>36</v>
       </c>
       <c r="G17">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="H17">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="I17">
         <v>1277</v>

</xml_diff>